<commit_message>
got ALL delete button semi working
</commit_message>
<xml_diff>
--- a/D3/Sprint #3 - Sprint Backlog.xlsx
+++ b/D3/Sprint #3 - Sprint Backlog.xlsx
@@ -342,6 +342,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -350,9 +353,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,7 +733,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -745,10 +745,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17"/>
       <c r="C1" s="1">
         <v>42319</v>
       </c>
@@ -822,7 +822,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -864,7 +864,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1">
-      <c r="A4" s="18"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
@@ -904,7 +904,7 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="18"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
@@ -944,7 +944,7 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
@@ -984,15 +984,15 @@
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="18"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
       </c>
-      <c r="D7" s="19">
-        <v>2</v>
+      <c r="D7" s="16">
+        <v>3</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -1020,11 +1020,11 @@
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1064,7 +1064,7 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="D12" s="11">
         <f t="shared" ref="D12:L12" si="3">SUM(D3:D10)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E12" s="11">
         <f t="shared" si="3"/>
@@ -1190,7 +1190,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="11">
         <f>B14</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O12" s="15"/>
     </row>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="B14" s="14">
         <f>SUM(N3:N10)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1"/>

</xml_diff>

<commit_message>
Delete All button sends message if successful or unsuccessful, created function for user input
</commit_message>
<xml_diff>
--- a/D3/Sprint #3 - Sprint Backlog.xlsx
+++ b/D3/Sprint #3 - Sprint Backlog.xlsx
@@ -733,7 +733,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -994,8 +994,8 @@
       <c r="D7" s="16">
         <v>3</v>
       </c>
-      <c r="E7" s="3">
-        <v>0</v>
+      <c r="E7" s="16">
+        <v>0.75</v>
       </c>
       <c r="F7" s="3">
         <v>0</v>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1113,8 +1113,8 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="6">
-        <v>0</v>
+      <c r="E10" s="16">
+        <v>0.25</v>
       </c>
       <c r="F10" s="6">
         <v>0</v>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="N10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="E12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="11">
         <f t="shared" si="3"/>
@@ -1190,7 +1190,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="11">
         <f>B14</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O12" s="15"/>
     </row>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="B14" s="14">
         <f>SUM(N3:N10)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1"/>

</xml_diff>

<commit_message>
added multiple tag support, working with delete all of one tag
</commit_message>
<xml_diff>
--- a/D3/Sprint #3 - Sprint Backlog.xlsx
+++ b/D3/Sprint #3 - Sprint Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <r>
       <rPr>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Total Work</t>
+  </si>
+  <si>
+    <t>Task #8: Implement a function to return list of multiple tags</t>
   </si>
 </sst>
 </file>
@@ -372,7 +375,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table5212" displayName="Table5212" ref="B2:L10" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table5212" displayName="Table5212" ref="B2:L11" headerRowCount="0">
   <tableColumns count="11">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -391,7 +394,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table8313" displayName="Table8313" ref="N2:N10" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table8313" displayName="Table8313" ref="N2:N11" headerRowCount="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1">
       <calculatedColumnFormula>SUM(C2:L2)</calculatedColumnFormula>
@@ -733,7 +736,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -899,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N10" si="1">SUM(C4:L4)</f>
+        <f t="shared" ref="N4:N11" si="1">SUM(C4:L4)</f>
         <v>0</v>
       </c>
     </row>
@@ -1142,63 +1145,104 @@
         <v>1.25</v>
       </c>
     </row>
+    <row r="11" spans="1:15">
+      <c r="B11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="16">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="9" t="s">
+      <c r="O12" s="15"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11">
-        <f t="shared" ref="C12" si="2">SUM(C3:C10)</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="11">
-        <f t="shared" ref="D12:L12" si="3">SUM(D3:D10)</f>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11">
+        <f>SUM(C3:C10)</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="11">
+        <f>SUM(D3:D10)</f>
         <v>4</v>
       </c>
-      <c r="E12" s="11">
-        <f t="shared" si="3"/>
+      <c r="E13" s="11">
+        <f>SUM(E3:E10)</f>
         <v>1</v>
       </c>
-      <c r="F12" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="3"/>
-      <c r="N12" s="11">
-        <f>B14</f>
+      <c r="F13" s="11">
+        <f>SUM(F3:F10)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <f>SUM(G3:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <f>SUM(H3:H10)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
+        <f>SUM(I3:I10)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="11">
+        <f>SUM(J3:J10)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="11">
+        <f>SUM(K3:K10)</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="11">
+        <f>SUM(L3:L10)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="11">
+        <f>B15</f>
         <v>5</v>
       </c>
-      <c r="O12" s="15"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="13" t="s">
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B15" s="14">
         <f>SUM(N3:N10)</f>
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
forgot to update sprint backlog
</commit_message>
<xml_diff>
--- a/D3/Sprint #3 - Sprint Backlog.xlsx
+++ b/D3/Sprint #3 - Sprint Backlog.xlsx
@@ -736,7 +736,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1040,8 +1040,8 @@
       <c r="E8" s="3">
         <v>0</v>
       </c>
-      <c r="F8" s="3">
-        <v>0</v>
+      <c r="F8" s="16">
+        <v>2</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="N8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1193,49 +1193,49 @@
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="11">
-        <f>SUM(C3:C10)</f>
+        <f t="shared" ref="C13:L13" si="2">SUM(C3:C10)</f>
         <v>0</v>
       </c>
       <c r="D13" s="11">
-        <f>SUM(D3:D10)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E13" s="11">
-        <f>SUM(E3:E10)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F13" s="11">
-        <f>SUM(F3:F10)</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="G13" s="12">
-        <f>SUM(G3:G10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H13" s="11">
-        <f>SUM(H3:H10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I13" s="11">
-        <f>SUM(I3:I10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J13" s="11">
-        <f>SUM(J3:J10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K13" s="11">
-        <f>SUM(K3:K10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L13" s="11">
-        <f>SUM(L3:L10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="11">
         <f>B15</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B15" s="14">
         <f>SUM(N3:N10)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1"/>

</xml_diff>